<commit_message>
Add 17zwd.com, bao66.cn, 3e3e.cn, 2tong.cn support
</commit_message>
<xml_diff>
--- a/poi-excel-core/src/main/resources/9.30.xlsx
+++ b/poi-excel-core/src/main/resources/9.30.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20344"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schen\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sc30\IdeaProjects\poiexcel\poi-excel-core\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7220896D-F443-4E23-A93A-BC1FB3B774EB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23280" windowHeight="10350"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23280" windowHeight="10350" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="4284    齐9.4部5.18" sheetId="1" r:id="rId1"/>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="86">
   <si>
     <t>商品价格：45.00 </t>
   </si>
@@ -252,13 +253,40 @@
   </si>
   <si>
     <t>http://www.k3.cn/p/iiiiboeaiim.html?_page=5&amp;_cat=new&amp;_pos=13&amp;_type=img?form=k3_detail</t>
+  </si>
+  <si>
+    <t>ERROR</t>
+  </si>
+  <si>
+    <t>https://gz.17zwd.com/item.htm?GID=108249029&amp;spm=0.42.137.11716.108249029.0&amp;action=0</t>
+  </si>
+  <si>
+    <t>https://gz.17zwd.com/item.htm?GID=100962686&amp;spm=0.42.137.11716.100962686.0&amp;action=0</t>
+  </si>
+  <si>
+    <t>http://www.bao66.cn/p/eubapui.html</t>
+  </si>
+  <si>
+    <t>http://www.bao66.cn/p/euebbad.html</t>
+  </si>
+  <si>
+    <t>http://www.3e3e.cn/product/oemcomo.html</t>
+  </si>
+  <si>
+    <t>http://www.3e3e.cn/product/oasogsq.html</t>
+  </si>
+  <si>
+    <t>http://www.2tong.cn/p/eoefmei.html</t>
+  </si>
+  <si>
+    <t>http://www.2tong.cn/p/aeboofp.html</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -302,6 +330,14 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -341,7 +377,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="28">
+  <cellStyleXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
@@ -394,8 +430,11 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -408,36 +447,43 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="28" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="28">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="28">
-    <cellStyle name="Excel Built-in Normal" xfId="3"/>
+  <cellStyles count="29">
+    <cellStyle name="Excel Built-in Normal" xfId="3" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Hyperlink" xfId="28" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="常规 10" xfId="6"/>
-    <cellStyle name="常规 11" xfId="8"/>
-    <cellStyle name="常规 12" xfId="2"/>
-    <cellStyle name="常规 13" xfId="9"/>
-    <cellStyle name="常规 14" xfId="10"/>
-    <cellStyle name="常规 15" xfId="11"/>
-    <cellStyle name="常规 16" xfId="4"/>
-    <cellStyle name="常规 17" xfId="13"/>
-    <cellStyle name="常规 18" xfId="14"/>
-    <cellStyle name="常规 19" xfId="15"/>
-    <cellStyle name="常规 2" xfId="16"/>
-    <cellStyle name="常规 2 2" xfId="5"/>
-    <cellStyle name="常规 2 3" xfId="7"/>
-    <cellStyle name="常规 20" xfId="12"/>
-    <cellStyle name="常规 3" xfId="17"/>
-    <cellStyle name="常规 3 2" xfId="18"/>
-    <cellStyle name="常规 3 3" xfId="19"/>
-    <cellStyle name="常规 4" xfId="20"/>
-    <cellStyle name="常规 4 2" xfId="21"/>
-    <cellStyle name="常规 4 3" xfId="22"/>
-    <cellStyle name="常规 5" xfId="23"/>
-    <cellStyle name="常规 6" xfId="1"/>
-    <cellStyle name="常规 7" xfId="24"/>
-    <cellStyle name="常规 8" xfId="25"/>
-    <cellStyle name="常规 9" xfId="26"/>
-    <cellStyle name="注释 2" xfId="27"/>
+    <cellStyle name="常规 10" xfId="6" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="常规 11" xfId="8" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="常规 12" xfId="2" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="常规 13" xfId="9" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="常规 14" xfId="10" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="常规 15" xfId="11" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="常规 16" xfId="4" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="常规 17" xfId="13" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
+    <cellStyle name="常规 18" xfId="14" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
+    <cellStyle name="常规 19" xfId="15" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
+    <cellStyle name="常规 2" xfId="16" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
+    <cellStyle name="常规 2 2" xfId="5" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
+    <cellStyle name="常规 2 3" xfId="7" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
+    <cellStyle name="常规 20" xfId="12" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
+    <cellStyle name="常规 3" xfId="17" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
+    <cellStyle name="常规 3 2" xfId="18" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
+    <cellStyle name="常规 3 3" xfId="19" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
+    <cellStyle name="常规 4" xfId="20" xr:uid="{00000000-0005-0000-0000-000013000000}"/>
+    <cellStyle name="常规 4 2" xfId="21" xr:uid="{00000000-0005-0000-0000-000014000000}"/>
+    <cellStyle name="常规 4 3" xfId="22" xr:uid="{00000000-0005-0000-0000-000015000000}"/>
+    <cellStyle name="常规 5" xfId="23" xr:uid="{00000000-0005-0000-0000-000016000000}"/>
+    <cellStyle name="常规 6" xfId="1" xr:uid="{00000000-0005-0000-0000-000017000000}"/>
+    <cellStyle name="常规 7" xfId="24" xr:uid="{00000000-0005-0000-0000-000018000000}"/>
+    <cellStyle name="常规 8" xfId="25" xr:uid="{00000000-0005-0000-0000-000019000000}"/>
+    <cellStyle name="常规 9" xfId="26" xr:uid="{00000000-0005-0000-0000-00001A000000}"/>
+    <cellStyle name="注释 2" xfId="27" xr:uid="{00000000-0005-0000-0000-00001B000000}"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
@@ -726,11 +772,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:E21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A2:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.95" customHeight="1"/>
@@ -814,45 +860,36 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="15.95" customHeight="1">
-      <c r="A6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C6" t="s">
-        <v>13</v>
-      </c>
       <c r="D6" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>30</v>
+        <v>77</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15.95" customHeight="1">
       <c r="A7" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B7" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C7" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>29</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15.95" customHeight="1">
       <c r="A8" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B8" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C8" t="s">
         <v>33</v>
@@ -861,266 +898,338 @@
         <v>29</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15.95" customHeight="1">
       <c r="A9" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B9" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C9" t="s">
-        <v>2</v>
+        <v>33</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>29</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15.95" customHeight="1">
       <c r="A10" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B10" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C10" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>29</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15.95" customHeight="1">
       <c r="A11" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B11" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C11" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>29</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15.95" customHeight="1">
       <c r="A12" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B12" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C12" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>29</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="15.95" customHeight="1">
       <c r="A13" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B13" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C13" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>29</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15.95" customHeight="1">
       <c r="A14" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B14" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C14" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>29</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="15.95" customHeight="1">
       <c r="A15" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B15" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C15" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>29</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="15.95" customHeight="1">
       <c r="A16" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B16" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C16" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>29</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="15.95" customHeight="1">
       <c r="A17" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B17" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C17" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>29</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="15.95" customHeight="1">
       <c r="A18" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B18" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C18" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>29</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="15.95" customHeight="1">
       <c r="A19" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B19" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C19" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>29</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="15.95" customHeight="1">
       <c r="A20" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B20" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C20" t="s">
-        <v>33</v>
+        <v>11</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>29</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="15.95" customHeight="1">
       <c r="A21" t="s">
+        <v>71</v>
+      </c>
+      <c r="B21" t="s">
+        <v>72</v>
+      </c>
+      <c r="C21" t="s">
+        <v>33</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="15.95" customHeight="1">
+      <c r="A22" t="s">
         <v>74</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B22" t="s">
         <v>75</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C22" t="s">
         <v>10</v>
       </c>
-      <c r="D21" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E21" s="3" t="s">
+      <c r="D22" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E22" s="3" t="s">
         <v>76</v>
       </c>
     </row>
+    <row r="23" spans="1:5" ht="15.95" customHeight="1">
+      <c r="E23" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="15.95" customHeight="1">
+      <c r="E24" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="15.95" customHeight="1">
+      <c r="E25" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="15.95" customHeight="1">
+      <c r="E26" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="15.95" customHeight="1">
+      <c r="E27" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="15.95" customHeight="1">
+      <c r="E28" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="15.95" customHeight="1">
+      <c r="E29" s="5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="15.95" customHeight="1">
+      <c r="E30" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="15.95" customHeight="1">
+      <c r="E31" s="5" t="s">
+        <v>85</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState ref="A1:I1043">
-    <sortCondition ref="F1:F1043"/>
+  <sortState ref="A1:I1044">
+    <sortCondition ref="F1:F1044"/>
   </sortState>
   <phoneticPr fontId="6" type="noConversion"/>
-  <conditionalFormatting sqref="A22:A1048576">
+  <conditionalFormatting sqref="A23:A1048576">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" tooltip="https://supplierportal.litb.cn/products/javascript:void(0);"/>
-    <hyperlink ref="A3" r:id="rId2" tooltip="https://supplierportal.litb.cn/products/javascript:void(0);"/>
-    <hyperlink ref="A4" r:id="rId3" tooltip="https://supplierportal.litb.cn/products/javascript:void(0);"/>
-    <hyperlink ref="A5" r:id="rId4" tooltip="https://supplierportal.litb.cn/products/javascript:void(0);"/>
-    <hyperlink ref="A6" r:id="rId5" tooltip="https://supplierportal.litb.cn/products/javascript:void(0);"/>
-    <hyperlink ref="A7" r:id="rId6" tooltip="https://supplierportal.litb.cn/products/javascript:void(0);"/>
-    <hyperlink ref="A8" r:id="rId7" tooltip="https://supplierportal.litb.cn/products/javascript:void(0);"/>
-    <hyperlink ref="A9" r:id="rId8" tooltip="https://supplierportal.litb.cn/products/javascript:void(0);"/>
-    <hyperlink ref="A10" r:id="rId9" tooltip="https://supplierportal.litb.cn/products/javascript:void(0);"/>
-    <hyperlink ref="A11" r:id="rId10" tooltip="https://supplierportal.litb.cn/products/javascript:void(0);"/>
-    <hyperlink ref="A12" r:id="rId11" tooltip="https://supplierportal.litb.cn/products/javascript:void(0);"/>
-    <hyperlink ref="A13" r:id="rId12" tooltip="https://supplierportal.litb.cn/products/javascript:void(0);"/>
-    <hyperlink ref="A14" r:id="rId13" tooltip="https://supplierportal.litb.cn/products/javascript:void(0);"/>
-    <hyperlink ref="A15" r:id="rId14" tooltip="https://supplierportal.litb.cn/products/javascript:void(0);"/>
-    <hyperlink ref="A16" r:id="rId15" tooltip="https://supplierportal.litb.cn/products/javascript:void(0);"/>
-    <hyperlink ref="A17" r:id="rId16" tooltip="https://supplierportal.litb.cn/products/javascript:void(0);"/>
-    <hyperlink ref="A18" r:id="rId17" tooltip="https://supplierportal.litb.cn/products/javascript:void(0);"/>
-    <hyperlink ref="A19" r:id="rId18" tooltip="https://supplierportal.litb.cn/products/javascript:void(0);"/>
-    <hyperlink ref="A20" r:id="rId19" tooltip="https://supplierportal.litb.cn/products/javascript:void(0);"/>
-    <hyperlink ref="A21" r:id="rId20" tooltip="https://supplierportal.litb.cn/products/javascript:void(0);"/>
+    <hyperlink ref="A2" r:id="rId1" tooltip="https://supplierportal.litb.cn/products/javascript:void(0);" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="A3" r:id="rId2" tooltip="https://supplierportal.litb.cn/products/javascript:void(0);" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="A4" r:id="rId3" tooltip="https://supplierportal.litb.cn/products/javascript:void(0);" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="A5" r:id="rId4" tooltip="https://supplierportal.litb.cn/products/javascript:void(0);" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="A7" r:id="rId5" tooltip="https://supplierportal.litb.cn/products/javascript:void(0);" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="A8" r:id="rId6" tooltip="https://supplierportal.litb.cn/products/javascript:void(0);" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="A9" r:id="rId7" tooltip="https://supplierportal.litb.cn/products/javascript:void(0);" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="A10" r:id="rId8" tooltip="https://supplierportal.litb.cn/products/javascript:void(0);" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="A11" r:id="rId9" tooltip="https://supplierportal.litb.cn/products/javascript:void(0);" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="A12" r:id="rId10" tooltip="https://supplierportal.litb.cn/products/javascript:void(0);" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="A13" r:id="rId11" tooltip="https://supplierportal.litb.cn/products/javascript:void(0);" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="A14" r:id="rId12" tooltip="https://supplierportal.litb.cn/products/javascript:void(0);" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="A15" r:id="rId13" tooltip="https://supplierportal.litb.cn/products/javascript:void(0);" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="A16" r:id="rId14" tooltip="https://supplierportal.litb.cn/products/javascript:void(0);" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="A17" r:id="rId15" tooltip="https://supplierportal.litb.cn/products/javascript:void(0);" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="A18" r:id="rId16" tooltip="https://supplierportal.litb.cn/products/javascript:void(0);" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="A19" r:id="rId17" tooltip="https://supplierportal.litb.cn/products/javascript:void(0);" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="A20" r:id="rId18" tooltip="https://supplierportal.litb.cn/products/javascript:void(0);" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="A21" r:id="rId19" tooltip="https://supplierportal.litb.cn/products/javascript:void(0);" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="A22" r:id="rId20" tooltip="https://supplierportal.litb.cn/products/javascript:void(0);" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="E6" r:id="rId21" xr:uid="{A3D45371-7D10-43B1-89FD-76EFA89B0BB6}"/>
+    <hyperlink ref="E23" r:id="rId22" xr:uid="{C84D97BD-F8D3-48E1-982D-F62CB18B6E6A}"/>
+    <hyperlink ref="E24" r:id="rId23" xr:uid="{21858916-3B52-4928-B435-0681583BA843}"/>
+    <hyperlink ref="E25" r:id="rId24" xr:uid="{161A6087-6F62-494B-B3F0-700593EBF34B}"/>
+    <hyperlink ref="E26" r:id="rId25" xr:uid="{11AC3770-C1D4-4FCD-816F-320917440748}"/>
+    <hyperlink ref="E27" r:id="rId26" xr:uid="{104884D0-9C49-41C8-998F-C6DBB3064ABA}"/>
+    <hyperlink ref="E28" r:id="rId27" xr:uid="{BAE84BCA-C81C-422F-B7A2-EED24E5BDD72}"/>
+    <hyperlink ref="E29" r:id="rId28" xr:uid="{A2974390-F5BF-4D64-857A-CCC24DC8E0D3}"/>
+    <hyperlink ref="E30" r:id="rId29" xr:uid="{B406B23A-0334-4D46-B29E-71AA046C512B}"/>
+    <hyperlink ref="E31" r:id="rId30" xr:uid="{69D5539A-7DD0-438D-B4E9-3A716F8AF33B}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1133,7 +1242,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>